<commit_message>
pam and total chl a data, scripts, and figures
</commit_message>
<xml_diff>
--- a/Carbamazepine/Data/PAM.xlsx
+++ b/Carbamazepine/Data/PAM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4795f5e3347afba5/Desktop/Dissertation/Lake_Murray/2024-25_Lake_Murray_Bioassays/Carbamazepine/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A47DC378-950F-42BC-BF74-53EF9E8AD2DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{A47DC378-950F-42BC-BF74-53EF9E8AD2DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{02BA8857-AF33-4568-BF5B-8567B5B387D2}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{643559BF-886C-4288-9EE2-F0D3242382D1}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{643559BF-886C-4288-9EE2-F0D3242382D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -480,7 +480,7 @@
   <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -524,6 +524,9 @@
       <c r="E2" t="s">
         <v>13</v>
       </c>
+      <c r="F2">
+        <v>0.48599999999999999</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
@@ -541,6 +544,9 @@
       <c r="E3" t="s">
         <v>14</v>
       </c>
+      <c r="F3">
+        <v>0.46200000000000002</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
@@ -558,6 +564,9 @@
       <c r="E4" t="s">
         <v>15</v>
       </c>
+      <c r="F4">
+        <v>0.45500000000000002</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
@@ -575,6 +584,9 @@
       <c r="E5" t="s">
         <v>16</v>
       </c>
+      <c r="F5">
+        <v>0.47499999999999998</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
@@ -591,6 +603,9 @@
       </c>
       <c r="E6" t="s">
         <v>17</v>
+      </c>
+      <c r="F6">
+        <v>0.46800000000000003</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>